<commit_message>
更新 PreModel.py 更新 ConfigHeadList.py 更新 ConfigInput.py 更新 ConfigRowData.py
</commit_message>
<xml_diff>
--- a/邻线干扰参数输入_20230509_鄂尔多斯.xlsx
+++ b/邻线干扰参数输入_20230509_鄂尔多斯.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\李继隆\PycharmProjects\Calculator_ZN_mix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD79C68D-F430-46EE-8B6E-B007EE7FE0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FEA3FE-0C69-427B-9010-F0FEE93BF6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I3"/>
+      <selection activeCell="Q2" sqref="Q2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -794,7 +794,7 @@
         <v>13</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R2">
         <v>46</v>
@@ -907,7 +907,7 @@
         <v>13</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>46</v>

</xml_diff>